<commit_message>
Created the template for student details and logic to fetch student details from database
</commit_message>
<xml_diff>
--- a/marks.xlsx
+++ b/marks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>stu_full_name</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>stu_sub5</t>
+  </si>
+  <si>
+    <t>Amjad Hussain</t>
   </si>
 </sst>
 </file>
@@ -404,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -449,261 +452,27 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B2">
-        <v>12345</v>
+        <v>12356</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2">
+        <v>65</v>
+      </c>
+      <c r="E2">
+        <v>85</v>
+      </c>
+      <c r="F2">
         <v>96</v>
       </c>
-      <c r="E2">
-        <v>97</v>
-      </c>
-      <c r="F2">
-        <v>92</v>
-      </c>
       <c r="G2">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="H2">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>12346</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>44</v>
-      </c>
-      <c r="E3">
-        <v>42</v>
-      </c>
-      <c r="F3">
-        <v>33</v>
-      </c>
-      <c r="G3">
-        <v>29</v>
-      </c>
-      <c r="H3">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>12347</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>55</v>
-      </c>
-      <c r="E4">
-        <v>56</v>
-      </c>
-      <c r="F4">
-        <v>50</v>
-      </c>
-      <c r="G4">
-        <v>49</v>
-      </c>
-      <c r="H4">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>12348</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>66</v>
-      </c>
-      <c r="E5">
-        <v>68</v>
-      </c>
-      <c r="F5">
-        <v>60</v>
-      </c>
-      <c r="G5">
-        <v>58</v>
-      </c>
-      <c r="H5">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>12349</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>88</v>
-      </c>
-      <c r="E6">
-        <v>89</v>
-      </c>
-      <c r="F6">
-        <v>80</v>
-      </c>
-      <c r="G6">
-        <v>75</v>
-      </c>
-      <c r="H6">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>12350</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7">
-        <v>98</v>
-      </c>
-      <c r="E7">
-        <v>92</v>
-      </c>
-      <c r="F7">
-        <v>90</v>
-      </c>
-      <c r="G7">
-        <v>96</v>
-      </c>
-      <c r="H7">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>12351</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>90</v>
-      </c>
-      <c r="E8">
-        <v>92</v>
-      </c>
-      <c r="F8">
-        <v>99</v>
-      </c>
-      <c r="G8">
-        <v>96</v>
-      </c>
-      <c r="H8">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <v>12352</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9">
-        <v>85</v>
-      </c>
-      <c r="E9">
-        <v>87</v>
-      </c>
-      <c r="F9">
-        <v>87</v>
-      </c>
-      <c r="G9">
-        <v>84</v>
-      </c>
-      <c r="H9">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10">
-        <v>12353</v>
-      </c>
-      <c r="C10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10">
-        <v>77</v>
-      </c>
-      <c r="E10">
-        <v>70</v>
-      </c>
-      <c r="F10">
-        <v>74</v>
-      </c>
-      <c r="G10">
-        <v>71</v>
-      </c>
-      <c r="H10">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
-        <v>12354</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11">
-        <v>70</v>
-      </c>
-      <c r="E11">
-        <v>70</v>
-      </c>
-      <c r="F11">
-        <v>71</v>
-      </c>
-      <c r="G11">
-        <v>65</v>
-      </c>
-      <c r="H11">
         <v>66</v>
       </c>
     </row>
@@ -715,14 +484,275 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:L1"/>
+      <selection sqref="A1:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1">
+        <v>12345</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>96</v>
+      </c>
+      <c r="E1">
+        <v>97</v>
+      </c>
+      <c r="F1">
+        <v>92</v>
+      </c>
+      <c r="G1">
+        <v>91</v>
+      </c>
+      <c r="H1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>12346</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>44</v>
+      </c>
+      <c r="E2">
+        <v>42</v>
+      </c>
+      <c r="F2">
+        <v>33</v>
+      </c>
+      <c r="G2">
+        <v>29</v>
+      </c>
+      <c r="H2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>12347</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>55</v>
+      </c>
+      <c r="E3">
+        <v>56</v>
+      </c>
+      <c r="F3">
+        <v>50</v>
+      </c>
+      <c r="G3">
+        <v>49</v>
+      </c>
+      <c r="H3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>12348</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>66</v>
+      </c>
+      <c r="E4">
+        <v>68</v>
+      </c>
+      <c r="F4">
+        <v>60</v>
+      </c>
+      <c r="G4">
+        <v>58</v>
+      </c>
+      <c r="H4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>12349</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>88</v>
+      </c>
+      <c r="E5">
+        <v>89</v>
+      </c>
+      <c r="F5">
+        <v>80</v>
+      </c>
+      <c r="G5">
+        <v>75</v>
+      </c>
+      <c r="H5">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>12350</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>98</v>
+      </c>
+      <c r="E6">
+        <v>92</v>
+      </c>
+      <c r="F6">
+        <v>90</v>
+      </c>
+      <c r="G6">
+        <v>96</v>
+      </c>
+      <c r="H6">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>12351</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>90</v>
+      </c>
+      <c r="E7">
+        <v>92</v>
+      </c>
+      <c r="F7">
+        <v>99</v>
+      </c>
+      <c r="G7">
+        <v>96</v>
+      </c>
+      <c r="H7">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>12352</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>85</v>
+      </c>
+      <c r="E8">
+        <v>87</v>
+      </c>
+      <c r="F8">
+        <v>87</v>
+      </c>
+      <c r="G8">
+        <v>84</v>
+      </c>
+      <c r="H8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>12353</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>77</v>
+      </c>
+      <c r="E9">
+        <v>70</v>
+      </c>
+      <c r="F9">
+        <v>74</v>
+      </c>
+      <c r="G9">
+        <v>71</v>
+      </c>
+      <c r="H9">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>12354</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>70</v>
+      </c>
+      <c r="E10">
+        <v>70</v>
+      </c>
+      <c r="F10">
+        <v>71</v>
+      </c>
+      <c r="G10">
+        <v>65</v>
+      </c>
+      <c r="H10">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added the functionality for bulk update student details and their marksheet data
</commit_message>
<xml_diff>
--- a/marks.xlsx
+++ b/marks.xlsx
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="21">
   <si>
     <t>stu_full_name</t>
   </si>
   <si>
-    <t>stu_class</t>
-  </si>
-  <si>
     <t>stu_roll_no</t>
   </si>
   <si>
@@ -76,6 +73,12 @@
   </si>
   <si>
     <t>Amjad Hussain</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>stu_semester</t>
   </si>
 </sst>
 </file>
@@ -407,21 +410,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="8.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -429,50 +429,310 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>17</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>12345</v>
+      </c>
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="B2">
+      <c r="D2">
+        <v>96</v>
+      </c>
+      <c r="E2">
+        <v>97</v>
+      </c>
+      <c r="F2">
+        <v>92</v>
+      </c>
+      <c r="G2">
+        <v>91</v>
+      </c>
+      <c r="H2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>12346</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>44</v>
+      </c>
+      <c r="E3">
+        <v>42</v>
+      </c>
+      <c r="F3">
+        <v>33</v>
+      </c>
+      <c r="G3">
+        <v>29</v>
+      </c>
+      <c r="H3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>12347</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>55</v>
+      </c>
+      <c r="E4">
+        <v>56</v>
+      </c>
+      <c r="F4">
+        <v>50</v>
+      </c>
+      <c r="G4">
+        <v>49</v>
+      </c>
+      <c r="H4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>12348</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>66</v>
+      </c>
+      <c r="E5">
+        <v>68</v>
+      </c>
+      <c r="F5">
+        <v>60</v>
+      </c>
+      <c r="G5">
+        <v>58</v>
+      </c>
+      <c r="H5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>12349</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>88</v>
+      </c>
+      <c r="E6">
+        <v>89</v>
+      </c>
+      <c r="F6">
+        <v>80</v>
+      </c>
+      <c r="G6">
+        <v>75</v>
+      </c>
+      <c r="H6">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>12350</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>98</v>
+      </c>
+      <c r="E7">
+        <v>92</v>
+      </c>
+      <c r="F7">
+        <v>90</v>
+      </c>
+      <c r="G7">
+        <v>96</v>
+      </c>
+      <c r="H7">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>12351</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>90</v>
+      </c>
+      <c r="E8">
+        <v>92</v>
+      </c>
+      <c r="F8">
+        <v>99</v>
+      </c>
+      <c r="G8">
+        <v>96</v>
+      </c>
+      <c r="H8">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>12352</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>85</v>
+      </c>
+      <c r="E9">
+        <v>87</v>
+      </c>
+      <c r="F9">
+        <v>87</v>
+      </c>
+      <c r="G9">
+        <v>84</v>
+      </c>
+      <c r="H9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>12353</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10">
+        <v>77</v>
+      </c>
+      <c r="E10">
+        <v>70</v>
+      </c>
+      <c r="F10">
+        <v>74</v>
+      </c>
+      <c r="G10">
+        <v>71</v>
+      </c>
+      <c r="H10">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>12354</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>70</v>
+      </c>
+      <c r="E11">
+        <v>70</v>
+      </c>
+      <c r="F11">
+        <v>71</v>
+      </c>
+      <c r="G11">
+        <v>65</v>
+      </c>
+      <c r="H11">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
         <v>12356</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2">
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12">
         <v>65</v>
       </c>
-      <c r="E2">
+      <c r="E12">
         <v>85</v>
       </c>
-      <c r="F2">
+      <c r="F12">
         <v>96</v>
       </c>
-      <c r="G2">
+      <c r="G12">
         <v>66</v>
       </c>
-      <c r="H2">
+      <c r="H12">
         <v>66</v>
       </c>
     </row>
@@ -491,16 +751,22 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="3" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1">
         <v>12345</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1">
         <v>96</v>
@@ -520,13 +786,13 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>12346</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>44</v>
@@ -546,13 +812,13 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>12347</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>55</v>
@@ -572,13 +838,13 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>12348</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>66</v>
@@ -598,13 +864,13 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>12349</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5">
         <v>88</v>
@@ -624,13 +890,13 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>12350</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>98</v>
@@ -650,13 +916,13 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>12351</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7">
         <v>90</v>
@@ -676,13 +942,13 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>12352</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8">
         <v>85</v>
@@ -702,13 +968,13 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>12353</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9">
         <v>77</v>
@@ -728,13 +994,13 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>12354</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10">
         <v>70</v>

</xml_diff>